<commit_message>
Final code after updation
</commit_message>
<xml_diff>
--- a/resources/Data.xlsx
+++ b/resources/Data.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swapnil123.galande@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baramati@123</t>
   </si>
 </sst>
 </file>
@@ -208,10 +202,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
@@ -226,18 +220,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="swapnil123.galande@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Baramati@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>